<commit_message>
Updated Results file with each feature method ran solo.
Updated Results file using each feature extraction method individually: LBP, HOG, Color, Gabor.
</commit_message>
<xml_diff>
--- a/Results/ReportResults.xlsx
+++ b/Results/ReportResults.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denista\Desktop\Pers\Masters\Exercises\MachineLearning1stSem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D35E47-EC4A-4C37-A72C-87AF3E289CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D921E1-43C6-4CC3-94AB-B2CF1A5F910D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="2" xr2:uid="{A2D50F8C-3EB1-4F62-BF6F-E0B5B8E1087D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{A2D50F8C-3EB1-4F62-BF6F-E0B5B8E1087D}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
     <sheet name="Baseline" sheetId="2" r:id="rId2"/>
     <sheet name="Baseline+PCA" sheetId="3" r:id="rId3"/>
+    <sheet name="LBP" sheetId="4" r:id="rId4"/>
+    <sheet name="HOG" sheetId="5" r:id="rId5"/>
+    <sheet name="Color" sheetId="6" r:id="rId6"/>
+    <sheet name="Gabor" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="69">
   <si>
     <t>Accuracy</t>
   </si>
@@ -177,6 +181,128 @@
   <si>
     <t>[[821 179]
  [159 841]]</t>
+  </si>
+  <si>
+    <t>24/01/26 Trying LBP solo, ImageResizing not applied to it. All features used, StandardScaler.</t>
+  </si>
+  <si>
+    <t>[[676 324]
+[289 711]]</t>
+  </si>
+  <si>
+    <t>[[5000   0]
+ [0 5000]]</t>
+  </si>
+  <si>
+    <t>[[635 365] [302 698]]</t>
+  </si>
+  <si>
+    <t>[[3518 1482]       [ 971 4029]]</t>
+  </si>
+  <si>
+    <t>24/01/26 Trying HOG solo with PCA. All features used, StandardScaler.</t>
+  </si>
+  <si>
+    <t>[[743 257]
+ [304 696]]</t>
+  </si>
+  <si>
+    <t>[[766 234]
+ [277 723]]</t>
+  </si>
+  <si>
+    <t>[[4026  974]
+ [ 846 4154]]</t>
+  </si>
+  <si>
+    <t>[[678 322]
+ [236 764]]</t>
+  </si>
+  <si>
+    <t>[[688 312]
+ [232 768]]</t>
+  </si>
+  <si>
+    <t>[[4769  231]
+ [ 241 4759]]</t>
+  </si>
+  <si>
+    <t>[[796 204]
+ [169 831]]</t>
+  </si>
+  <si>
+    <t>[[803 197]
+ [169 831]]</t>
+  </si>
+  <si>
+    <t>24/01/26 Trying Color solo. All features used, StandardScaler.</t>
+  </si>
+  <si>
+    <t>[[571 429]
+ [469 531]]</t>
+  </si>
+  <si>
+    <t>[[564 436]
+ [483 517]]</t>
+  </si>
+  <si>
+    <t>[[3400 1600]
+ [2218 2782]]</t>
+  </si>
+  <si>
+    <t>[[621 379]
+ [522 478]]</t>
+  </si>
+  <si>
+    <t>[[605 395]
+ [508 492]]</t>
+  </si>
+  <si>
+    <t>[[2899 2101]
+ [2129 2871]]</t>
+  </si>
+  <si>
+    <t>[[550 450]
+ [438 562]]</t>
+  </si>
+  <si>
+    <t>[[584 416]
+ [450 550]]</t>
+  </si>
+  <si>
+    <t>24/01/26 Trying Gabor solo. All features used, StandardScaler.</t>
+  </si>
+  <si>
+    <t>[[544 456]
+ [499 501]]</t>
+  </si>
+  <si>
+    <t>[[581 419]
+ [506 494]]</t>
+  </si>
+  <si>
+    <t>[[3295 1705]
+ [2064 2936]]</t>
+  </si>
+  <si>
+    <t>[[585 415]
+ [480 520]]</t>
+  </si>
+  <si>
+    <t>[[608 392]
+ [468 532]]</t>
+  </si>
+  <si>
+    <t>[[3075 1925]
+ [2303 2697]]</t>
+  </si>
+  <si>
+    <t>[[590 410]
+ [469 531]]</t>
+  </si>
+  <si>
+    <t>[[615 385]
+ [468 532]]</t>
   </si>
 </sst>
 </file>
@@ -571,7 +697,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -749,7 +875,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -935,13 +1061,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2FEDAA-E607-4E26-9E52-F4CA8C65CD29}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="4" width="10.9140625" customWidth="1"/>
+    <col min="2" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.9140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -961,144 +1088,893 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
         <v>0.83550000000000002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>0.95909999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
         <v>0.83730000000000004</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>0.95909999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4">
         <v>0.73850000000000005</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>0.73099999999999998</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>0.83</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
         <v>0.73080000000000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>0.73880000000000001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>0.83220000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4">
         <v>0.73699999999999999</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>0.74</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>0.83099999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
         <v>0.73299999999999998</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>0.75019999999999998</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>0.8327</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47356A9C-EF8E-4EE4-A308-3151F10F48A2}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.75470000000000004</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.81840000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.76659999999999995</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.82550000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.69350000000000001</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.6845</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.69879999999999998</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.69650000000000001</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.78039999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="31.5" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.66649999999999998</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.73450000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.67669999999999997</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.67979999999999996</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.75009999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D8E866-08FF-4005-91CB-C7DDBC5BAAE0}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.08203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.95279999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.82030000000000003</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.95279999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.71950000000000003</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.8135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.7127</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.81669999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.74450000000000005</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.81699999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.7389</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.73850000000000005</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.81950000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3541AA1D-751F-45BD-8512-C586FCCA0D37}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.4140625" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.61819999999999997</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.59309999999999996</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.57579999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.54949999999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.54179999999999995</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.51480000000000004</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.55859999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.54049999999999998</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.54849999999999999</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.56699999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.52939999999999998</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.52149999999999996</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.5595</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06C64E8-54C4-44CA-BA40-FE177DA33079}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.4140625" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.62309999999999999</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.57720000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.60909999999999997</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.56059999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.52249999999999996</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.55249999999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.5605</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.54710000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.57350000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.51649999999999996</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LBP & HOG with PCA applied.
As expected, these two feature extraction methods have similar results as Baseline and Baseline with PCA applied but with faster computation.
</commit_message>
<xml_diff>
--- a/Results/ReportResults.xlsx
+++ b/Results/ReportResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denista\Desktop\Pers\Masters\Exercises\MachineLearning1stSem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D921E1-43C6-4CC3-94AB-B2CF1A5F910D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEF3B26-B2EB-4990-A8B3-AF4DCCE20DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{A2D50F8C-3EB1-4F62-BF6F-E0B5B8E1087D}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="7" xr2:uid="{A2D50F8C-3EB1-4F62-BF6F-E0B5B8E1087D}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="HOG" sheetId="5" r:id="rId5"/>
     <sheet name="Color" sheetId="6" r:id="rId6"/>
     <sheet name="Gabor" sheetId="7" r:id="rId7"/>
+    <sheet name="LBP+HOG" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="78">
   <si>
     <t>Accuracy</t>
   </si>
@@ -303,6 +304,41 @@
   <si>
     <t>[[615 385]
  [468 532]]</t>
+  </si>
+  <si>
+    <t>25/01/26 Trying LBP and HOG combined, ImageResizing not applied to LBP. All features used, StandardScaler. PCA Applied with 90% threshold.</t>
+  </si>
+  <si>
+    <t>[[750 250]
+ [285 715]]</t>
+  </si>
+  <si>
+    <t>[[743 257]
+ [260 740]]</t>
+  </si>
+  <si>
+    <t>[[4076  924]
+ [ 775 4225]]</t>
+  </si>
+  <si>
+    <t>[[692 308]
+ [248 752]]</t>
+  </si>
+  <si>
+    <t>[[691 309]
+ [221 779]]</t>
+  </si>
+  <si>
+    <t>[[4764  236]
+ [ 214 4786]]</t>
+  </si>
+  <si>
+    <t>[[806 194]
+ [149 851]]</t>
+  </si>
+  <si>
+    <t>[[815 185]
+ [153 847]]</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1098,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1247,7 +1283,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1430,7 +1466,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1613,7 +1649,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="A1:XFD1048576"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1799,7 +1835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06C64E8-54C4-44CA-BA40-FE177DA33079}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1980,4 +2016,207 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39452DFF-1386-4110-8CCE-17FC90835CF4}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="14.4140625" customWidth="1"/>
+    <col min="3" max="4" width="11.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.83009999999999995</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.83260000000000001</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.95509999999999995</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="28">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.73250000000000004</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.82850000000000001</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.72770000000000001</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.73009999999999997</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.83230000000000004</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="28">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.74150000000000005</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.74109999999999998</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.74619999999999997</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.8337</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="28">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>